<commit_message>
Deploying to gh-pages from  @ 79b1d25dae1d2c29af8b9c382c2182e78f56476b 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2023_5-1-2.xlsx
+++ b/assets/excel/2023_5-1-2.xlsx
@@ -5,17 +5,17 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15_Uebergreifende_Analysen\Projekte\Integrationsmonitoring_2023\Datentabellen\Downloadtabellen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15_Uebergreifende_Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9903852F-943E-41B4-9210-8F17D8C8E392}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DA26287-43A9-473D-A926-F5DBC47FABDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11208" xr2:uid="{7A929791-C940-4C1C-A1AE-0CA9018FEC89}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{4B6D923C-7796-4823-AE86-5D5E8D269325}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="28">
   <si>
     <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2023</t>
   </si>
@@ -446,9 +446,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -493,11 +490,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard_Tabelle_A_6_HT" xfId="2" xr:uid="{CF2B28C0-6EF9-412B-99A8-01908F137BFF}"/>
+    <cellStyle name="Standard_Tabelle_A_6_HT" xfId="2" xr:uid="{26B74755-C2E5-41AB-963F-93DF5EC13AA6}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -808,30 +808,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32AD47A9-BA67-4FEF-80D2-FFD928475FF1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFA28CB-5600-40E6-A819-F51D3073956E}">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:S61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" customWidth="1"/>
-    <col min="5" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="8" width="14.6640625" customWidth="1"/>
-    <col min="10" max="11" width="12.6640625" customWidth="1"/>
-    <col min="12" max="13" width="14.6640625" customWidth="1"/>
-    <col min="15" max="16" width="12.6640625" customWidth="1"/>
-    <col min="17" max="18" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="5" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="8" width="14.7109375" customWidth="1"/>
+    <col min="10" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="13" width="14.7109375" customWidth="1"/>
+    <col min="15" max="16" width="12.7109375" customWidth="1"/>
+    <col min="17" max="18" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -845,13 +845,13 @@
       <c r="J3" s="2"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="2:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -862,7 +862,7 @@
       <c r="I5" s="5"/>
       <c r="N5" s="7"/>
     </row>
-    <row r="6" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
@@ -891,7 +891,7 @@
       <c r="Q6" s="10"/>
       <c r="R6" s="11"/>
     </row>
-    <row r="7" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
       <c r="C7" s="13"/>
       <c r="D7" s="9" t="s">
@@ -922,7 +922,7 @@
       <c r="Q7" s="9"/>
       <c r="R7" s="14"/>
     </row>
-    <row r="8" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -959,7 +959,7 @@
       </c>
       <c r="R8" s="11"/>
     </row>
-    <row r="9" spans="2:19" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:19" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
       <c r="D9" s="17"/>
@@ -990,7 +990,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="21"/>
       <c r="C10" s="17"/>
       <c r="D10" s="10" t="s">
@@ -1012,7 +1012,7 @@
       <c r="R10" s="11"/>
       <c r="S10" s="7"/>
     </row>
-    <row r="11" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="22">
         <v>1</v>
       </c>
@@ -1066,2130 +1066,2130 @@
       </c>
       <c r="S11" s="24"/>
     </row>
-    <row r="12" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="25">
+    <row r="12" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="43">
         <v>2022</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="27">
-        <v>85.206887123479106</v>
-      </c>
-      <c r="E12" s="27">
-        <v>87.25383073808058</v>
-      </c>
-      <c r="F12" s="27">
-        <v>79.579049300788924</v>
-      </c>
-      <c r="G12" s="27">
-        <v>82.84871550903901</v>
-      </c>
-      <c r="H12" s="27">
-        <v>69.857975442765792</v>
-      </c>
-      <c r="I12" s="27">
-        <v>82.523582397885548</v>
-      </c>
-      <c r="J12" s="27">
-        <v>78.822382611581219</v>
-      </c>
-      <c r="K12" s="27">
-        <v>75.368118253538768</v>
-      </c>
-      <c r="L12" s="27">
-        <v>78.176974310180782</v>
-      </c>
-      <c r="M12" s="27">
-        <v>67.011825949188037</v>
-      </c>
-      <c r="N12" s="27">
-        <v>2.6833047255935472</v>
-      </c>
-      <c r="O12" s="27">
-        <v>2.1272959830976288</v>
-      </c>
-      <c r="P12" s="27">
+      <c r="D12" s="26">
+        <v>82.291935655370409</v>
+      </c>
+      <c r="E12" s="26">
+        <v>83.780144892262925</v>
+      </c>
+      <c r="F12" s="26">
+        <v>78.200563925835198</v>
+      </c>
+      <c r="G12" s="26">
+        <v>81.320647002854415</v>
+      </c>
+      <c r="H12" s="26">
+        <v>68.918689526396207</v>
+      </c>
+      <c r="I12" s="26">
+        <v>79.624960126380387</v>
+      </c>
+      <c r="J12" s="26">
+        <v>81.675116126125673</v>
+      </c>
+      <c r="K12" s="26">
+        <v>73.98963287858507</v>
+      </c>
+      <c r="L12" s="26">
+        <v>76.6489058039962</v>
+      </c>
+      <c r="M12" s="26">
+        <v>66.072540032818424</v>
+      </c>
+      <c r="N12" s="26">
+        <v>2.6669755289900201</v>
+      </c>
+      <c r="O12" s="26">
+        <v>2.1050287661372593</v>
+      </c>
+      <c r="P12" s="26">
         <v>4.2109310472501491</v>
       </c>
-      <c r="Q12" s="27">
+      <c r="Q12" s="26">
         <v>4.6717411988582302</v>
       </c>
-      <c r="R12" s="27">
+      <c r="R12" s="26">
         <v>2.8404911446839809</v>
       </c>
       <c r="S12" s="24"/>
     </row>
-    <row r="13" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="25">
+    <row r="13" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="43">
         <v>2022</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="27">
-        <v>76.296969183750448</v>
-      </c>
-      <c r="E13" s="27">
-        <v>80.442695370831245</v>
-      </c>
-      <c r="F13" s="27">
-        <v>64.349956673738305</v>
-      </c>
-      <c r="G13" s="27">
-        <v>63.952939324781624</v>
-      </c>
-      <c r="H13" s="27">
-        <v>65.606954361999371</v>
-      </c>
-      <c r="I13" s="27">
-        <v>74.420511320333489</v>
-      </c>
-      <c r="J13" s="27">
-        <v>78.822382611581219</v>
-      </c>
-      <c r="K13" s="27">
-        <v>61.736934891086733</v>
-      </c>
-      <c r="L13" s="27">
-        <v>61.192649720626427</v>
-      </c>
-      <c r="M13" s="27">
-        <v>63.458553244334063</v>
-      </c>
-      <c r="N13" s="27">
-        <v>1.8764578634169624</v>
-      </c>
-      <c r="O13" s="27">
-        <v>1.6208312593330017</v>
-      </c>
-      <c r="P13" s="27">
-        <v>2.6130217826515669</v>
-      </c>
-      <c r="Q13" s="27">
-        <v>2.7602896041551901</v>
-      </c>
-      <c r="R13" s="27">
+      <c r="D13" s="26">
+        <v>74.308501220178755</v>
+      </c>
+      <c r="E13" s="26">
+        <v>78.088186494109834</v>
+      </c>
+      <c r="F13" s="26">
+        <v>63.417695042878066</v>
+      </c>
+      <c r="G13" s="26">
+        <v>62.874793420949082</v>
+      </c>
+      <c r="H13" s="26">
+        <v>65.135051226327221</v>
+      </c>
+      <c r="I13" s="26">
+        <v>72.455523137206598</v>
+      </c>
+      <c r="J13" s="26">
+        <v>76.494835739173723</v>
+      </c>
+      <c r="K13" s="26">
+        <v>60.816625332417004</v>
+      </c>
+      <c r="L13" s="26">
+        <v>60.130243173054218</v>
+      </c>
+      <c r="M13" s="26">
+        <v>62.986650108661898</v>
+      </c>
+      <c r="N13" s="26">
+        <v>1.8529780829721554</v>
+      </c>
+      <c r="O13" s="26">
+        <v>1.5933507549361208</v>
+      </c>
+      <c r="P13" s="26">
+        <v>2.6010697104610512</v>
+      </c>
+      <c r="Q13" s="26">
+        <v>2.7445502478948609</v>
+      </c>
+      <c r="R13" s="26">
         <v>2.1484011176653208</v>
       </c>
       <c r="S13" s="24"/>
     </row>
-    <row r="14" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="25">
+    <row r="14" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="43">
         <v>2022</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="27">
-        <v>80.782178009630513</v>
-      </c>
-      <c r="E14" s="27">
-        <v>83.85042477064458</v>
-      </c>
-      <c r="F14" s="27">
-        <v>72.147773338388404</v>
-      </c>
-      <c r="G14" s="27">
-        <v>73.558203873164501</v>
-      </c>
-      <c r="H14" s="27">
-        <v>67.831132689916515</v>
-      </c>
-      <c r="I14" s="27">
+      <c r="D14" s="26">
+        <v>78.327334175700443</v>
+      </c>
+      <c r="E14" s="26">
+        <v>80.936231290789777</v>
+      </c>
+      <c r="F14" s="26">
+        <v>70.986322144127854</v>
+      </c>
+      <c r="G14" s="26">
+        <v>72.251349416703746</v>
+      </c>
+      <c r="H14" s="26">
+        <v>67.114690034933986</v>
+      </c>
+      <c r="I14" s="26">
         <v>78.499567028400264</v>
       </c>
-      <c r="J14" s="27">
-        <v>81.976200407800548</v>
-      </c>
-      <c r="K14" s="27">
-        <v>68.715914724838882</v>
-      </c>
-      <c r="L14" s="27">
-        <v>69.826268645166294</v>
-      </c>
-      <c r="M14" s="27">
-        <v>65.317662383800112</v>
-      </c>
-      <c r="N14" s="27">
-        <v>2.2824198237910727</v>
-      </c>
-      <c r="O14" s="27">
-        <v>1.8742243628440334</v>
-      </c>
-      <c r="P14" s="27">
-        <v>3.4311295167546447</v>
-      </c>
-      <c r="Q14" s="27">
-        <v>3.7319352279982199</v>
-      </c>
-      <c r="R14" s="27">
+      <c r="J14" s="26">
+        <v>79.086620048552618</v>
+      </c>
+      <c r="K14" s="26">
+        <v>67.560296304937452</v>
+      </c>
+      <c r="L14" s="26">
+        <v>68.52715277912128</v>
+      </c>
+      <c r="M14" s="26">
+        <v>64.601219728817583</v>
+      </c>
+      <c r="N14" s="26">
+        <v>2.2627306075556892</v>
+      </c>
+      <c r="O14" s="26">
+        <v>1.8493521567570788</v>
+      </c>
+      <c r="P14" s="26">
+        <v>3.4260258391904115</v>
+      </c>
+      <c r="Q14" s="26">
+        <v>3.7241966375824642</v>
+      </c>
+      <c r="R14" s="26">
         <v>2.5105097992776368</v>
       </c>
       <c r="S14" s="24"/>
     </row>
-    <row r="15" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="25">
+    <row r="15" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="43">
         <v>2021</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="27">
-        <v>83.769472065295176</v>
-      </c>
-      <c r="E15" s="27">
-        <v>85.835447663258009</v>
-      </c>
-      <c r="F15" s="27">
-        <v>77.898354661791586</v>
-      </c>
-      <c r="G15" s="27">
-        <v>80.761347581238937</v>
-      </c>
-      <c r="H15" s="27">
-        <v>69.959165655004966</v>
-      </c>
-      <c r="I15" s="27">
-        <v>80.594554674057036</v>
-      </c>
-      <c r="J15" s="27">
-        <v>76.193075885085662</v>
-      </c>
-      <c r="K15" s="27">
-        <v>72.813162705667281</v>
-      </c>
-      <c r="L15" s="27">
-        <v>75.444252084452671</v>
-      </c>
-      <c r="M15" s="27">
-        <v>65.517051098112788</v>
-      </c>
-      <c r="N15" s="27">
-        <v>3.1745367056996239</v>
-      </c>
-      <c r="O15" s="27">
-        <v>2.5022001039581285</v>
-      </c>
-      <c r="P15" s="27">
-        <v>5.0851919561243148</v>
-      </c>
-      <c r="Q15" s="27">
-        <v>5.317095496786262</v>
-      </c>
-      <c r="R15" s="27">
-        <v>4.442114556892176</v>
+      <c r="D15" s="26">
+        <v>81.116474547364888</v>
+      </c>
+      <c r="E15" s="26">
+        <v>82.685310510578518</v>
+      </c>
+      <c r="F15" s="26">
+        <v>76.658135283363805</v>
+      </c>
+      <c r="G15" s="26">
+        <v>79.436053568941162</v>
+      </c>
+      <c r="H15" s="26">
+        <v>68.954861494316305</v>
+      </c>
+      <c r="I15" s="26">
+        <v>77.97391542690076</v>
+      </c>
+      <c r="J15" s="26">
+        <v>80.213474414463562</v>
+      </c>
+      <c r="K15" s="26">
+        <v>71.609506398537476</v>
+      </c>
+      <c r="L15" s="26">
+        <v>74.150796967345229</v>
+      </c>
+      <c r="M15" s="26">
+        <v>64.556892175256593</v>
+      </c>
+      <c r="N15" s="26">
+        <v>3.1425591204641314</v>
+      </c>
+      <c r="O15" s="26">
+        <v>2.4718360961149513</v>
+      </c>
+      <c r="P15" s="26">
+        <v>5.0486288848263259</v>
+      </c>
+      <c r="Q15" s="26">
+        <v>5.2852566015959246</v>
+      </c>
+      <c r="R15" s="26">
+        <v>4.3979693190597065</v>
       </c>
       <c r="S15" s="24"/>
     </row>
-    <row r="16" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="25">
+    <row r="16" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="43">
         <v>2021</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="27">
-        <v>74.124601209373807</v>
-      </c>
-      <c r="E16" s="27">
-        <v>78.016295670625567</v>
-      </c>
-      <c r="F16" s="27">
-        <v>62.222012222012225</v>
-      </c>
-      <c r="G16" s="27">
-        <v>62.119194097376372</v>
-      </c>
-      <c r="H16" s="27">
-        <v>62.522388981532949</v>
-      </c>
-      <c r="I16" s="27">
-        <v>71.973266473642951</v>
-      </c>
-      <c r="J16" s="27">
-        <v>76.193075885085662</v>
-      </c>
-      <c r="K16" s="27">
-        <v>59.067284067284064</v>
-      </c>
-      <c r="L16" s="27">
-        <v>58.806367730069141</v>
-      </c>
-      <c r="M16" s="27">
-        <v>59.835711197578902</v>
-      </c>
-      <c r="N16" s="27">
-        <v>2.1513347357308641</v>
-      </c>
-      <c r="O16" s="27">
-        <v>1.8232197855399102</v>
-      </c>
-      <c r="P16" s="27">
-        <v>3.1547281547281552</v>
-      </c>
-      <c r="Q16" s="27">
-        <v>3.3128263673072449</v>
-      </c>
-      <c r="R16" s="27">
-        <v>2.6928540547217592</v>
+      <c r="D16" s="26">
+        <v>72.589208783872948</v>
+      </c>
+      <c r="E16" s="26">
+        <v>76.227583152213114</v>
+      </c>
+      <c r="F16" s="26">
+        <v>61.462861462861476</v>
+      </c>
+      <c r="G16" s="26">
+        <v>61.262975412781962</v>
+      </c>
+      <c r="H16" s="26">
+        <v>62.046816132419245</v>
+      </c>
+      <c r="I16" s="26">
+        <v>70.447188865688091</v>
+      </c>
+      <c r="J16" s="26">
+        <v>74.407453569699527</v>
+      </c>
+      <c r="K16" s="26">
+        <v>58.334908334908341</v>
+      </c>
+      <c r="L16" s="26">
+        <v>57.967062007145728</v>
+      </c>
+      <c r="M16" s="26">
+        <v>59.409548514606882</v>
+      </c>
+      <c r="N16" s="26">
+        <v>2.1424080355826032</v>
+      </c>
+      <c r="O16" s="26">
+        <v>1.8196145486758482</v>
+      </c>
+      <c r="P16" s="26">
+        <v>3.1279531279531279</v>
+      </c>
+      <c r="Q16" s="26">
+        <v>3.2959134056362442</v>
+      </c>
+      <c r="R16" s="26">
+        <v>2.6372676178123644</v>
       </c>
       <c r="S16" s="24"/>
     </row>
-    <row r="17" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="25">
+    <row r="17" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="43">
         <v>2021</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="27">
-        <v>78.993461942045357</v>
-      </c>
-      <c r="E17" s="27">
-        <v>81.927351076399518</v>
-      </c>
-      <c r="F17" s="27">
-        <v>70.350428841180886</v>
-      </c>
-      <c r="G17" s="27">
-        <v>71.722328146462473</v>
-      </c>
-      <c r="H17" s="27">
-        <v>66.450033514994317</v>
-      </c>
-      <c r="I17" s="27">
+      <c r="D17" s="26">
+        <v>76.894057324277682</v>
+      </c>
+      <c r="E17" s="26">
+        <v>79.457668654803058</v>
+      </c>
+      <c r="F17" s="26">
+        <v>69.341836850766299</v>
+      </c>
+      <c r="G17" s="26">
+        <v>70.624474649937468</v>
+      </c>
+      <c r="H17" s="26">
+        <v>65.695217556028325</v>
+      </c>
+      <c r="I17" s="26">
         <v>76.325580680250155</v>
       </c>
-      <c r="J17" s="27">
-        <v>79.764512666325146</v>
-      </c>
-      <c r="K17" s="27">
-        <v>66.194726504735826</v>
-      </c>
-      <c r="L17" s="27">
-        <v>67.377042458535783</v>
-      </c>
-      <c r="M17" s="27">
-        <v>62.833328476087779</v>
-      </c>
-      <c r="N17" s="27">
-        <v>2.6678812617952175</v>
-      </c>
-      <c r="O17" s="27">
-        <v>2.1628384100743685</v>
-      </c>
-      <c r="P17" s="27">
-        <v>4.1557023364450538</v>
-      </c>
-      <c r="Q17" s="27">
-        <v>4.3452856879266877</v>
-      </c>
-      <c r="R17" s="27">
-        <v>3.6167050389065372</v>
+      <c r="J17" s="26">
+        <v>77.311819929930422</v>
+      </c>
+      <c r="K17" s="26">
+        <v>65.217984787702761</v>
+      </c>
+      <c r="L17" s="26">
+        <v>66.303790721036563</v>
+      </c>
+      <c r="M17" s="26">
+        <v>62.130970769096258</v>
+      </c>
+      <c r="N17" s="26">
+        <v>2.6473177050301921</v>
+      </c>
+      <c r="O17" s="26">
+        <v>2.1458487248726414</v>
+      </c>
+      <c r="P17" s="26">
+        <v>4.124610402905958</v>
+      </c>
+      <c r="Q17" s="26">
+        <v>4.3206839289009169</v>
+      </c>
+      <c r="R17" s="26">
+        <v>3.5671611342639817</v>
       </c>
       <c r="S17" s="24"/>
     </row>
-    <row r="18" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="26">
+    <row r="18" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="25">
         <v>2019</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="27">
+      <c r="D18" s="26">
         <v>83.03</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="26">
         <v>84.49</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="26">
         <v>78.47</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="26">
         <v>81.790000000000006</v>
       </c>
-      <c r="H18" s="27">
+      <c r="H18" s="26">
         <v>61.64</v>
       </c>
-      <c r="I18" s="27">
+      <c r="I18" s="26">
         <v>80</v>
       </c>
-      <c r="J18" s="27">
+      <c r="J18" s="26">
         <v>82.12</v>
       </c>
-      <c r="K18" s="27">
+      <c r="K18" s="26">
         <v>73.38</v>
       </c>
-      <c r="L18" s="27">
+      <c r="L18" s="26">
         <v>76.55</v>
       </c>
-      <c r="M18" s="27">
+      <c r="M18" s="26">
         <v>56.92</v>
       </c>
-      <c r="N18" s="27">
+      <c r="N18" s="26">
         <v>3.03</v>
       </c>
-      <c r="O18" s="27">
+      <c r="O18" s="26">
         <v>2.37</v>
       </c>
-      <c r="P18" s="27">
+      <c r="P18" s="26">
         <v>5.09</v>
       </c>
-      <c r="Q18" s="27">
+      <c r="Q18" s="26">
         <v>5.24</v>
       </c>
-      <c r="R18" s="27">
+      <c r="R18" s="26">
         <v>4.71</v>
       </c>
       <c r="S18" s="24"/>
     </row>
-    <row r="19" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="26">
+    <row r="19" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="25">
         <v>2019</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="26">
         <v>73.760000000000005</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E19" s="26">
         <v>76.930000000000007</v>
       </c>
-      <c r="F19" s="27">
+      <c r="F19" s="26">
         <v>62.96</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="26">
         <v>63.49</v>
       </c>
-      <c r="H19" s="27">
+      <c r="H19" s="26">
         <v>52.55</v>
       </c>
-      <c r="I19" s="27">
+      <c r="I19" s="26">
         <v>71.849999999999994</v>
       </c>
-      <c r="J19" s="27">
+      <c r="J19" s="26">
         <v>75.37</v>
       </c>
-      <c r="K19" s="27">
+      <c r="K19" s="26">
         <v>59.83</v>
       </c>
-      <c r="L19" s="27">
+      <c r="L19" s="26">
         <v>60.43</v>
       </c>
-      <c r="M19" s="27">
+      <c r="M19" s="26">
         <v>48.56</v>
       </c>
-      <c r="N19" s="27">
+      <c r="N19" s="26">
         <v>1.91</v>
       </c>
-      <c r="O19" s="27">
+      <c r="O19" s="26">
         <v>1.55</v>
       </c>
-      <c r="P19" s="27">
+      <c r="P19" s="26">
         <v>3.13</v>
       </c>
-      <c r="Q19" s="27">
+      <c r="Q19" s="26">
         <v>3.06</v>
       </c>
-      <c r="R19" s="27">
+      <c r="R19" s="26">
         <v>3.99</v>
       </c>
       <c r="S19" s="24"/>
     </row>
-    <row r="20" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="26">
+    <row r="20" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="25">
         <v>2019</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D20" s="26">
         <v>78.459999999999994</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="26">
         <v>80.72</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F20" s="26">
         <v>71.08</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="26">
         <v>73.02</v>
       </c>
-      <c r="H20" s="27">
+      <c r="H20" s="26">
         <v>57.54</v>
       </c>
-      <c r="I20" s="27">
+      <c r="I20" s="26">
         <v>75.98</v>
       </c>
-      <c r="J20" s="27">
+      <c r="J20" s="26">
         <v>78.75</v>
       </c>
-      <c r="K20" s="27">
+      <c r="K20" s="26">
         <v>66.92</v>
       </c>
-      <c r="L20" s="27">
+      <c r="L20" s="26">
         <v>68.83</v>
       </c>
-      <c r="M20" s="27">
+      <c r="M20" s="26">
         <v>53.15</v>
       </c>
-      <c r="N20" s="27">
+      <c r="N20" s="26">
         <v>2.48</v>
       </c>
-      <c r="O20" s="27">
+      <c r="O20" s="26">
         <v>1.96</v>
       </c>
-      <c r="P20" s="27">
+      <c r="P20" s="26">
         <v>4.16</v>
       </c>
-      <c r="Q20" s="27">
+      <c r="Q20" s="26">
         <v>4.2</v>
       </c>
-      <c r="R20" s="27">
+      <c r="R20" s="26">
         <v>4.3899999999999997</v>
       </c>
       <c r="S20" s="24"/>
     </row>
-    <row r="21" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="28">
+    <row r="21" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="27">
         <v>2018</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="29">
+      <c r="D21" s="28">
         <v>82.14</v>
       </c>
-      <c r="E21" s="29">
+      <c r="E21" s="28">
         <v>83.7</v>
       </c>
-      <c r="F21" s="29">
+      <c r="F21" s="28">
         <v>76.77</v>
       </c>
-      <c r="G21" s="29">
+      <c r="G21" s="28">
         <v>80.5</v>
       </c>
-      <c r="H21" s="29">
+      <c r="H21" s="28">
         <v>60.37</v>
       </c>
-      <c r="I21" s="29">
+      <c r="I21" s="28">
         <v>79.08</v>
       </c>
-      <c r="J21" s="29">
+      <c r="J21" s="28">
         <v>81.22</v>
       </c>
-      <c r="K21" s="29">
+      <c r="K21" s="28">
         <v>71.7</v>
       </c>
-      <c r="L21" s="29">
+      <c r="L21" s="28">
         <v>75.22</v>
       </c>
-      <c r="M21" s="29">
+      <c r="M21" s="28">
         <v>56.17</v>
       </c>
-      <c r="N21" s="29">
+      <c r="N21" s="28">
         <v>3.06</v>
       </c>
-      <c r="O21" s="29">
+      <c r="O21" s="28">
         <v>2.48</v>
       </c>
-      <c r="P21" s="29">
+      <c r="P21" s="28">
         <v>5.08</v>
       </c>
-      <c r="Q21" s="29">
+      <c r="Q21" s="28">
         <v>5.27</v>
       </c>
-      <c r="R21" s="29">
+      <c r="R21" s="28">
         <v>4.2</v>
       </c>
-      <c r="S21" s="30"/>
-    </row>
-    <row r="22" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="28">
+      <c r="S21" s="29"/>
+    </row>
+    <row r="22" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="27">
         <v>2018</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="29">
+      <c r="D22" s="28">
         <v>73.53</v>
       </c>
-      <c r="E22" s="29">
+      <c r="E22" s="28">
         <v>76.650000000000006</v>
       </c>
-      <c r="F22" s="29">
+      <c r="F22" s="28">
         <v>61.86</v>
       </c>
-      <c r="G22" s="29">
+      <c r="G22" s="28">
         <v>63.85</v>
       </c>
-      <c r="H22" s="29">
+      <c r="H22" s="28">
         <v>52.14</v>
       </c>
-      <c r="I22" s="29">
+      <c r="I22" s="28">
         <v>71.38</v>
       </c>
-      <c r="J22" s="29">
+      <c r="J22" s="28">
         <v>74.78</v>
       </c>
-      <c r="K22" s="29">
+      <c r="K22" s="28">
         <v>58.62</v>
       </c>
-      <c r="L22" s="29">
+      <c r="L22" s="28">
         <v>60.77</v>
       </c>
-      <c r="M22" s="29">
+      <c r="M22" s="28">
         <v>48.17</v>
       </c>
-      <c r="N22" s="29">
+      <c r="N22" s="28">
         <v>2.15</v>
       </c>
-      <c r="O22" s="29">
+      <c r="O22" s="28">
         <v>1.87</v>
       </c>
-      <c r="P22" s="29">
+      <c r="P22" s="28">
         <v>3.23</v>
       </c>
-      <c r="Q22" s="29">
+      <c r="Q22" s="28">
         <v>3.08</v>
       </c>
-      <c r="R22" s="29">
+      <c r="R22" s="28">
         <v>3.97</v>
       </c>
-      <c r="S22" s="30"/>
-    </row>
-    <row r="23" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="28">
+      <c r="S22" s="29"/>
+    </row>
+    <row r="23" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="27">
         <v>2018</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="29">
+      <c r="D23" s="28">
         <v>77.91</v>
       </c>
-      <c r="E23" s="29">
+      <c r="E23" s="28">
         <v>80.2</v>
       </c>
-      <c r="F23" s="29">
+      <c r="F23" s="28">
         <v>69.680000000000007</v>
       </c>
-      <c r="G23" s="29">
+      <c r="G23" s="28">
         <v>72.510000000000005</v>
       </c>
-      <c r="H23" s="29">
+      <c r="H23" s="28">
         <v>56.62</v>
       </c>
-      <c r="I23" s="29">
+      <c r="I23" s="28">
         <v>75.290000000000006</v>
       </c>
-      <c r="J23" s="29">
+      <c r="J23" s="28">
         <v>78.03</v>
       </c>
-      <c r="K23" s="29">
+      <c r="K23" s="28">
         <v>65.48</v>
       </c>
-      <c r="L23" s="29">
+      <c r="L23" s="28">
         <v>68.290000000000006</v>
       </c>
-      <c r="M23" s="29">
+      <c r="M23" s="28">
         <v>52.53</v>
       </c>
-      <c r="N23" s="29">
+      <c r="N23" s="28">
         <v>2.62</v>
       </c>
-      <c r="O23" s="29">
+      <c r="O23" s="28">
         <v>2.1800000000000002</v>
       </c>
-      <c r="P23" s="29">
+      <c r="P23" s="28">
         <v>4.2</v>
       </c>
-      <c r="Q23" s="29">
+      <c r="Q23" s="28">
         <v>4.22</v>
       </c>
-      <c r="R23" s="29">
+      <c r="R23" s="28">
         <v>4.0999999999999996</v>
       </c>
-      <c r="S23" s="30"/>
-    </row>
-    <row r="24" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="28">
+      <c r="S23" s="29"/>
+    </row>
+    <row r="24" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="27">
         <v>2017</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="29">
+      <c r="D24" s="28">
         <v>81.61</v>
       </c>
-      <c r="E24" s="29">
+      <c r="E24" s="28">
         <v>83.41</v>
       </c>
-      <c r="F24" s="29">
+      <c r="F24" s="28">
         <v>75.95</v>
       </c>
-      <c r="G24" s="29">
+      <c r="G24" s="28">
         <v>78.459999999999994</v>
       </c>
-      <c r="H24" s="29">
+      <c r="H24" s="28">
         <v>60.8</v>
       </c>
-      <c r="I24" s="29">
+      <c r="I24" s="28">
         <v>78.13</v>
       </c>
-      <c r="J24" s="29">
+      <c r="J24" s="28">
         <v>80.69</v>
       </c>
-      <c r="K24" s="29">
+      <c r="K24" s="28">
         <v>70.09</v>
       </c>
-      <c r="L24" s="29">
+      <c r="L24" s="28">
         <v>72.44</v>
       </c>
-      <c r="M24" s="29">
+      <c r="M24" s="28">
         <v>54.88</v>
       </c>
-      <c r="N24" s="29">
+      <c r="N24" s="28">
         <v>3.48</v>
       </c>
-      <c r="O24" s="29">
+      <c r="O24" s="28">
         <v>2.72</v>
       </c>
-      <c r="P24" s="29">
+      <c r="P24" s="28">
         <v>5.85</v>
       </c>
-      <c r="Q24" s="29">
+      <c r="Q24" s="28">
         <v>6.02</v>
       </c>
-      <c r="R24" s="29">
+      <c r="R24" s="28">
         <v>5.92</v>
       </c>
-      <c r="S24" s="30"/>
-    </row>
-    <row r="25" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="28">
+      <c r="S24" s="29"/>
+    </row>
+    <row r="25" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="27">
         <v>2017</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="29">
+      <c r="D25" s="28">
         <v>72.73</v>
       </c>
-      <c r="E25" s="29">
+      <c r="E25" s="28">
         <v>75.900000000000006</v>
       </c>
-      <c r="F25" s="29">
+      <c r="F25" s="28">
         <v>61.84</v>
       </c>
-      <c r="G25" s="29">
+      <c r="G25" s="28">
         <v>62.82</v>
       </c>
-      <c r="H25" s="29">
+      <c r="H25" s="28">
         <v>50.81</v>
       </c>
-      <c r="I25" s="29">
+      <c r="I25" s="28">
         <v>70.3</v>
       </c>
-      <c r="J25" s="29">
+      <c r="J25" s="28">
         <v>73.900000000000006</v>
       </c>
-      <c r="K25" s="29">
+      <c r="K25" s="28">
         <v>57.93</v>
       </c>
-      <c r="L25" s="29">
+      <c r="L25" s="28">
         <v>58.84</v>
       </c>
-      <c r="M25" s="29">
+      <c r="M25" s="28">
         <v>46.49</v>
       </c>
-      <c r="N25" s="29">
+      <c r="N25" s="28">
         <v>2.4300000000000002</v>
       </c>
-      <c r="O25" s="29">
+      <c r="O25" s="28">
         <v>2</v>
       </c>
-      <c r="P25" s="29">
+      <c r="P25" s="28">
         <v>3.91</v>
       </c>
-      <c r="Q25" s="29">
+      <c r="Q25" s="28">
         <v>3.98</v>
       </c>
-      <c r="R25" s="29">
+      <c r="R25" s="28">
         <v>4.32</v>
       </c>
-      <c r="S25" s="30"/>
-    </row>
-    <row r="26" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="28">
+      <c r="S25" s="29"/>
+    </row>
+    <row r="26" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="27">
         <v>2017</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="29">
+      <c r="D26" s="28">
         <v>77.260000000000005</v>
       </c>
-      <c r="E26" s="29">
+      <c r="E26" s="28">
         <v>79.69</v>
       </c>
-      <c r="F26" s="29">
+      <c r="F26" s="28">
         <v>69.27</v>
       </c>
-      <c r="G26" s="29">
+      <c r="G26" s="28">
         <v>71.040000000000006</v>
       </c>
-      <c r="H26" s="29">
+      <c r="H26" s="28">
         <v>56.25</v>
       </c>
-      <c r="I26" s="29">
+      <c r="I26" s="28">
         <v>74.290000000000006</v>
       </c>
-      <c r="J26" s="29">
+      <c r="J26" s="28">
         <v>77.33</v>
       </c>
-      <c r="K26" s="29">
+      <c r="K26" s="28">
         <v>64.34</v>
       </c>
-      <c r="L26" s="29">
+      <c r="L26" s="28">
         <v>65.989999999999995</v>
       </c>
-      <c r="M26" s="29">
+      <c r="M26" s="28">
         <v>51.05</v>
       </c>
-      <c r="N26" s="29">
+      <c r="N26" s="28">
         <v>2.96</v>
       </c>
-      <c r="O26" s="29">
+      <c r="O26" s="28">
         <v>2.36</v>
       </c>
-      <c r="P26" s="29">
+      <c r="P26" s="28">
         <v>4.93</v>
       </c>
-      <c r="Q26" s="29">
+      <c r="Q26" s="28">
         <v>5.05</v>
       </c>
-      <c r="R26" s="29">
+      <c r="R26" s="28">
         <v>5.19</v>
       </c>
-      <c r="S26" s="30"/>
-    </row>
-    <row r="27" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="28">
+      <c r="S26" s="29"/>
+    </row>
+    <row r="27" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="27">
         <v>2016</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D27" s="29">
+      <c r="D27" s="28">
         <v>81.13</v>
       </c>
-      <c r="E27" s="29">
+      <c r="E27" s="28">
         <v>82.69</v>
       </c>
-      <c r="F27" s="29">
+      <c r="F27" s="28">
         <v>75.3</v>
       </c>
-      <c r="G27" s="29">
+      <c r="G27" s="28">
         <v>78.64</v>
       </c>
-      <c r="H27" s="29">
+      <c r="H27" s="28">
         <v>59.98</v>
       </c>
-      <c r="I27" s="29">
+      <c r="I27" s="28">
         <v>77.319999999999993</v>
       </c>
-      <c r="J27" s="29">
+      <c r="J27" s="28">
         <v>79.59</v>
       </c>
-      <c r="K27" s="29">
+      <c r="K27" s="28">
         <v>68.83</v>
       </c>
-      <c r="L27" s="29">
+      <c r="L27" s="28">
         <v>72.349999999999994</v>
       </c>
-      <c r="M27" s="29">
+      <c r="M27" s="28">
         <v>52.69</v>
       </c>
-      <c r="N27" s="29">
+      <c r="N27" s="28">
         <v>3.81</v>
       </c>
-      <c r="O27" s="29">
+      <c r="O27" s="28">
         <v>3.1</v>
       </c>
-      <c r="P27" s="29">
+      <c r="P27" s="28">
         <v>6.47</v>
       </c>
-      <c r="Q27" s="29">
+      <c r="Q27" s="28">
         <v>6.29</v>
       </c>
-      <c r="R27" s="29">
+      <c r="R27" s="28">
         <v>7.29</v>
       </c>
-      <c r="S27" s="30"/>
-    </row>
-    <row r="28" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="28">
+      <c r="S27" s="29"/>
+    </row>
+    <row r="28" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="27">
         <v>2016</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="29">
+      <c r="D28" s="28">
         <v>71.459999999999994</v>
       </c>
-      <c r="E28" s="29">
+      <c r="E28" s="28">
         <v>74.22</v>
       </c>
-      <c r="F28" s="29">
+      <c r="F28" s="28">
         <v>60.19</v>
       </c>
-      <c r="G28" s="29">
+      <c r="G28" s="28">
         <v>62.56</v>
       </c>
-      <c r="H28" s="29">
+      <c r="H28" s="28">
         <v>47.99</v>
       </c>
-      <c r="I28" s="29">
+      <c r="I28" s="28">
         <v>69</v>
       </c>
-      <c r="J28" s="29">
+      <c r="J28" s="28">
         <v>72.010000000000005</v>
       </c>
-      <c r="K28" s="29">
+      <c r="K28" s="28">
         <v>56.69</v>
       </c>
-      <c r="L28" s="29">
+      <c r="L28" s="28">
         <v>59.06</v>
       </c>
-      <c r="M28" s="29">
+      <c r="M28" s="28">
         <v>44.46</v>
       </c>
-      <c r="N28" s="29">
+      <c r="N28" s="28">
         <v>2.46</v>
       </c>
-      <c r="O28" s="29">
+      <c r="O28" s="28">
         <v>2.2000000000000002</v>
       </c>
-      <c r="P28" s="29">
+      <c r="P28" s="28">
         <v>3.5</v>
       </c>
-      <c r="Q28" s="29">
+      <c r="Q28" s="28">
         <v>3.5</v>
       </c>
-      <c r="R28" s="29">
+      <c r="R28" s="28">
         <v>3.53</v>
       </c>
-      <c r="S28" s="30"/>
-    </row>
-    <row r="29" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="28">
+      <c r="S28" s="29"/>
+    </row>
+    <row r="29" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="27">
         <v>2016</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29" s="28">
         <v>76.38</v>
       </c>
-      <c r="E29" s="29">
+      <c r="E29" s="28">
         <v>78.489999999999995</v>
       </c>
-      <c r="F29" s="29">
+      <c r="F29" s="28">
         <v>68.150000000000006</v>
       </c>
-      <c r="G29" s="29">
+      <c r="G29" s="28">
         <v>70.95</v>
       </c>
-      <c r="H29" s="29">
+      <c r="H29" s="28">
         <v>54.58</v>
       </c>
-      <c r="I29" s="29">
+      <c r="I29" s="28">
         <v>73.23</v>
       </c>
-      <c r="J29" s="29">
+      <c r="J29" s="28">
         <v>75.83</v>
       </c>
-      <c r="K29" s="29">
+      <c r="K29" s="28">
         <v>63.08</v>
       </c>
-      <c r="L29" s="29">
+      <c r="L29" s="28">
         <v>65.989999999999995</v>
       </c>
-      <c r="M29" s="29">
+      <c r="M29" s="28">
         <v>48.99</v>
       </c>
-      <c r="N29" s="29">
+      <c r="N29" s="28">
         <v>3.15</v>
       </c>
-      <c r="O29" s="29">
+      <c r="O29" s="28">
         <v>2.65</v>
       </c>
-      <c r="P29" s="29">
+      <c r="P29" s="28">
         <v>5.07</v>
       </c>
-      <c r="Q29" s="29">
+      <c r="Q29" s="28">
         <v>4.96</v>
       </c>
-      <c r="R29" s="29">
+      <c r="R29" s="28">
         <v>5.6</v>
       </c>
-      <c r="S29" s="30"/>
-    </row>
-    <row r="30" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="28">
+      <c r="S29" s="29"/>
+    </row>
+    <row r="30" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="27">
         <v>2015</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="29">
+      <c r="D30" s="28">
         <v>81.400000000000006</v>
       </c>
-      <c r="E30" s="29">
+      <c r="E30" s="28">
         <v>82.38</v>
       </c>
-      <c r="F30" s="29">
+      <c r="F30" s="28">
         <v>77.13</v>
       </c>
-      <c r="G30" s="29">
+      <c r="G30" s="28">
         <v>81.93</v>
       </c>
-      <c r="H30" s="29">
+      <c r="H30" s="28">
         <v>55.23</v>
       </c>
-      <c r="I30" s="29">
+      <c r="I30" s="28">
         <v>77.599999999999994</v>
       </c>
-      <c r="J30" s="29">
+      <c r="J30" s="28">
         <v>79.03</v>
       </c>
-      <c r="K30" s="29">
+      <c r="K30" s="28">
         <v>71.38</v>
       </c>
-      <c r="L30" s="29">
+      <c r="L30" s="28">
         <v>76.2</v>
       </c>
-      <c r="M30" s="29">
+      <c r="M30" s="28">
         <v>49.39</v>
       </c>
-      <c r="N30" s="29">
+      <c r="N30" s="28">
         <v>3.8</v>
       </c>
-      <c r="O30" s="29">
+      <c r="O30" s="28">
         <v>3.36</v>
       </c>
-      <c r="P30" s="29">
+      <c r="P30" s="28">
         <v>5.75</v>
       </c>
-      <c r="Q30" s="29">
+      <c r="Q30" s="28">
         <v>5.73</v>
       </c>
-      <c r="R30" s="29">
+      <c r="R30" s="28">
         <v>5.84</v>
       </c>
-      <c r="S30" s="30"/>
-    </row>
-    <row r="31" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="28">
+      <c r="S30" s="29"/>
+    </row>
+    <row r="31" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="27">
         <v>2015</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="29">
+      <c r="D31" s="28">
         <v>71.95</v>
       </c>
-      <c r="E31" s="29">
+      <c r="E31" s="28">
         <v>74.430000000000007</v>
       </c>
-      <c r="F31" s="29">
+      <c r="F31" s="28">
         <v>61.02</v>
       </c>
-      <c r="G31" s="29">
+      <c r="G31" s="28">
         <v>64.28</v>
       </c>
-      <c r="H31" s="29">
+      <c r="H31" s="28">
         <v>43.78</v>
       </c>
-      <c r="I31" s="29">
+      <c r="I31" s="28">
         <v>69.099999999999994</v>
       </c>
-      <c r="J31" s="29">
+      <c r="J31" s="28">
         <v>71.930000000000007</v>
       </c>
-      <c r="K31" s="29">
+      <c r="K31" s="28">
         <v>56.65</v>
       </c>
-      <c r="L31" s="29">
+      <c r="L31" s="28">
         <v>59.66</v>
       </c>
-      <c r="M31" s="29">
+      <c r="M31" s="28">
         <v>40.72</v>
       </c>
-      <c r="N31" s="29">
+      <c r="N31" s="28">
         <v>2.85</v>
       </c>
-      <c r="O31" s="29">
+      <c r="O31" s="28">
         <v>2.5</v>
       </c>
-      <c r="P31" s="29">
+      <c r="P31" s="28">
         <v>4.37</v>
       </c>
-      <c r="Q31" s="29">
+      <c r="Q31" s="28">
         <v>4.62</v>
       </c>
-      <c r="R31" s="29">
+      <c r="R31" s="28">
         <v>3.06</v>
       </c>
-      <c r="S31" s="30"/>
-    </row>
-    <row r="32" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="28">
+      <c r="S31" s="29"/>
+    </row>
+    <row r="32" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="27">
         <v>2015</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="29">
+      <c r="D32" s="28">
         <v>76.709999999999994</v>
       </c>
-      <c r="E32" s="29">
+      <c r="E32" s="28">
         <v>78.430000000000007</v>
       </c>
-      <c r="F32" s="29">
+      <c r="F32" s="28">
         <v>69.17</v>
       </c>
-      <c r="G32" s="29">
+      <c r="G32" s="28">
         <v>73.09</v>
       </c>
-      <c r="H32" s="29">
+      <c r="H32" s="28">
         <v>49.92</v>
       </c>
-      <c r="I32" s="29">
+      <c r="I32" s="28">
         <v>73.38</v>
       </c>
-      <c r="J32" s="29">
+      <c r="J32" s="28">
         <v>75.5</v>
       </c>
-      <c r="K32" s="29">
+      <c r="K32" s="28">
         <v>64.099999999999994</v>
       </c>
-      <c r="L32" s="29">
+      <c r="L32" s="28">
         <v>67.92</v>
       </c>
-      <c r="M32" s="29">
+      <c r="M32" s="28">
         <v>45.37</v>
       </c>
-      <c r="N32" s="29">
+      <c r="N32" s="28">
         <v>3.33</v>
       </c>
-      <c r="O32" s="29">
+      <c r="O32" s="28">
         <v>2.93</v>
       </c>
-      <c r="P32" s="29">
+      <c r="P32" s="28">
         <v>5.07</v>
       </c>
-      <c r="Q32" s="29">
+      <c r="Q32" s="28">
         <v>5.17</v>
       </c>
-      <c r="R32" s="29">
+      <c r="R32" s="28">
         <v>4.55</v>
       </c>
-      <c r="S32" s="30"/>
-    </row>
-    <row r="33" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="28">
+      <c r="S32" s="29"/>
+    </row>
+    <row r="33" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="27">
         <v>2014</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="29">
+      <c r="D33" s="28">
         <v>82.1</v>
       </c>
-      <c r="E33" s="29">
+      <c r="E33" s="28">
         <v>83.01</v>
       </c>
-      <c r="F33" s="29">
+      <c r="F33" s="28">
         <v>78</v>
       </c>
-      <c r="G33" s="29">
+      <c r="G33" s="28">
         <v>83.32</v>
       </c>
-      <c r="H33" s="29">
+      <c r="H33" s="28">
         <v>54.37</v>
       </c>
-      <c r="I33" s="29">
+      <c r="I33" s="28">
         <v>77.849999999999994</v>
       </c>
-      <c r="J33" s="29">
+      <c r="J33" s="28">
         <v>79.19</v>
       </c>
-      <c r="K33" s="29">
+      <c r="K33" s="28">
         <v>71.77</v>
       </c>
-      <c r="L33" s="29">
+      <c r="L33" s="28">
         <v>76.75</v>
       </c>
-      <c r="M33" s="29">
+      <c r="M33" s="28">
         <v>49.65</v>
       </c>
-      <c r="N33" s="29">
+      <c r="N33" s="28">
         <v>4.26</v>
       </c>
-      <c r="O33" s="29">
+      <c r="O33" s="28">
         <v>3.82</v>
       </c>
-      <c r="P33" s="29">
+      <c r="P33" s="28">
         <v>6.23</v>
       </c>
-      <c r="Q33" s="29">
+      <c r="Q33" s="28">
         <v>6.57</v>
       </c>
-      <c r="R33" s="29">
+      <c r="R33" s="28">
         <v>4.72</v>
       </c>
-      <c r="S33" s="30"/>
-    </row>
-    <row r="34" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="28">
+      <c r="S33" s="29"/>
+    </row>
+    <row r="34" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="27">
         <v>2014</v>
       </c>
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="29">
+      <c r="D34" s="28">
         <v>71.739999999999995</v>
       </c>
-      <c r="E34" s="29">
+      <c r="E34" s="28">
         <v>74</v>
       </c>
-      <c r="F34" s="29">
+      <c r="F34" s="28">
         <v>61.62</v>
       </c>
-      <c r="G34" s="29">
+      <c r="G34" s="28">
         <v>65.09</v>
       </c>
-      <c r="H34" s="29">
+      <c r="H34" s="28">
         <v>44.17</v>
       </c>
-      <c r="I34" s="29">
+      <c r="I34" s="28">
         <v>68.73</v>
       </c>
-      <c r="J34" s="29">
+      <c r="J34" s="28">
         <v>71.31</v>
       </c>
-      <c r="K34" s="29">
+      <c r="K34" s="28">
         <v>57.17</v>
       </c>
-      <c r="L34" s="29">
+      <c r="L34" s="28">
         <v>60.58</v>
       </c>
-      <c r="M34" s="29">
+      <c r="M34" s="28">
         <v>40.03</v>
       </c>
-      <c r="N34" s="29">
+      <c r="N34" s="28">
         <v>3.01</v>
       </c>
-      <c r="O34" s="29">
+      <c r="O34" s="28">
         <v>2.69</v>
       </c>
-      <c r="P34" s="29">
+      <c r="P34" s="28">
         <v>4.45</v>
       </c>
-      <c r="Q34" s="29">
+      <c r="Q34" s="28">
         <v>4.5199999999999996</v>
       </c>
-      <c r="R34" s="29">
+      <c r="R34" s="28">
         <v>4.1399999999999997</v>
       </c>
-      <c r="S34" s="30"/>
-    </row>
-    <row r="35" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="28">
+      <c r="S34" s="29"/>
+    </row>
+    <row r="35" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="27">
         <v>2014</v>
       </c>
-      <c r="C35" s="28" t="s">
+      <c r="C35" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="29">
+      <c r="D35" s="28">
         <v>76.959999999999994</v>
       </c>
-      <c r="E35" s="29">
+      <c r="E35" s="28">
         <v>78.53</v>
       </c>
-      <c r="F35" s="29">
+      <c r="F35" s="28">
         <v>69.819999999999993</v>
       </c>
-      <c r="G35" s="29">
+      <c r="G35" s="28">
         <v>74.12</v>
       </c>
-      <c r="H35" s="29">
+      <c r="H35" s="28">
         <v>49.54</v>
       </c>
-      <c r="I35" s="29">
+      <c r="I35" s="28">
         <v>73.319999999999993</v>
       </c>
-      <c r="J35" s="29">
+      <c r="J35" s="28">
         <v>75.28</v>
       </c>
-      <c r="K35" s="29">
+      <c r="K35" s="28">
         <v>64.48</v>
       </c>
-      <c r="L35" s="29">
+      <c r="L35" s="28">
         <v>68.59</v>
       </c>
-      <c r="M35" s="29">
+      <c r="M35" s="28">
         <v>45.1</v>
       </c>
-      <c r="N35" s="29">
+      <c r="N35" s="28">
         <v>3.64</v>
       </c>
-      <c r="O35" s="29">
+      <c r="O35" s="28">
         <v>3.26</v>
       </c>
-      <c r="P35" s="29">
+      <c r="P35" s="28">
         <v>5.34</v>
       </c>
-      <c r="Q35" s="29">
+      <c r="Q35" s="28">
         <v>5.53</v>
       </c>
-      <c r="R35" s="29">
+      <c r="R35" s="28">
         <v>4.4400000000000004</v>
       </c>
-      <c r="S35" s="30"/>
-    </row>
-    <row r="36" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="28">
+      <c r="S35" s="29"/>
+    </row>
+    <row r="36" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="27">
         <v>2013</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="C36" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="29">
+      <c r="D36" s="28">
         <v>82.15</v>
       </c>
-      <c r="E36" s="29">
+      <c r="E36" s="28">
         <v>83.06</v>
       </c>
-      <c r="F36" s="29">
+      <c r="F36" s="28">
         <v>78.290000000000006</v>
       </c>
-      <c r="G36" s="29">
+      <c r="G36" s="28">
         <v>83.11</v>
       </c>
-      <c r="H36" s="29">
+      <c r="H36" s="28">
         <v>54.64</v>
       </c>
-      <c r="I36" s="29">
+      <c r="I36" s="28">
         <v>77.78</v>
       </c>
-      <c r="J36" s="29">
+      <c r="J36" s="28">
         <v>79.260000000000005</v>
       </c>
-      <c r="K36" s="29">
+      <c r="K36" s="28">
         <v>71.510000000000005</v>
       </c>
-      <c r="L36" s="29">
+      <c r="L36" s="28">
         <v>76.19</v>
       </c>
-      <c r="M36" s="29">
+      <c r="M36" s="28">
         <v>48.27</v>
       </c>
-      <c r="N36" s="29">
+      <c r="N36" s="28">
         <v>4.37</v>
       </c>
-      <c r="O36" s="29">
+      <c r="O36" s="28">
         <v>3.8</v>
       </c>
-      <c r="P36" s="29">
+      <c r="P36" s="28">
         <v>6.78</v>
       </c>
-      <c r="Q36" s="29">
+      <c r="Q36" s="28">
         <v>6.92</v>
       </c>
-      <c r="R36" s="29">
+      <c r="R36" s="28">
         <v>6.37</v>
       </c>
-      <c r="S36" s="30"/>
-    </row>
-    <row r="37" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="28">
+      <c r="S36" s="29"/>
+    </row>
+    <row r="37" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="27">
         <v>2013</v>
       </c>
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="29">
+      <c r="D37" s="28">
         <v>71.680000000000007</v>
       </c>
-      <c r="E37" s="29">
+      <c r="E37" s="28">
         <v>73.739999999999995</v>
       </c>
-      <c r="F37" s="29">
+      <c r="F37" s="28">
         <v>62.97</v>
       </c>
-      <c r="G37" s="29">
+      <c r="G37" s="28">
         <v>65.900000000000006</v>
       </c>
-      <c r="H37" s="29">
+      <c r="H37" s="28">
         <v>43.21</v>
       </c>
-      <c r="I37" s="29">
+      <c r="I37" s="28">
         <v>68.430000000000007</v>
       </c>
-      <c r="J37" s="29">
+      <c r="J37" s="28">
         <v>70.650000000000006</v>
       </c>
-      <c r="K37" s="29">
+      <c r="K37" s="28">
         <v>59.01</v>
       </c>
-      <c r="L37" s="29">
+      <c r="L37" s="28">
         <v>61.98</v>
       </c>
-      <c r="M37" s="29">
+      <c r="M37" s="28">
         <v>39.56</v>
       </c>
-      <c r="N37" s="29">
+      <c r="N37" s="28">
         <v>3.25</v>
       </c>
-      <c r="O37" s="29">
+      <c r="O37" s="28">
         <v>3.08</v>
       </c>
-      <c r="P37" s="29">
+      <c r="P37" s="28">
         <v>3.97</v>
       </c>
-      <c r="Q37" s="29">
+      <c r="Q37" s="28">
         <v>3.92</v>
       </c>
-      <c r="R37" s="29">
+      <c r="R37" s="28">
         <v>3.65</v>
       </c>
-      <c r="S37" s="30"/>
-    </row>
-    <row r="38" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="28">
+      <c r="S37" s="29"/>
+    </row>
+    <row r="38" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="27">
         <v>2013</v>
       </c>
-      <c r="C38" s="28" t="s">
+      <c r="C38" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="29">
+      <c r="D38" s="28">
         <v>76.930000000000007</v>
       </c>
-      <c r="E38" s="29">
+      <c r="E38" s="28">
         <v>78.42</v>
       </c>
-      <c r="F38" s="29">
+      <c r="F38" s="28">
         <v>70.66</v>
       </c>
-      <c r="G38" s="29">
+      <c r="G38" s="28">
         <v>74.45</v>
       </c>
-      <c r="H38" s="29">
+      <c r="H38" s="28">
         <v>49.25</v>
       </c>
-      <c r="I38" s="29">
+      <c r="I38" s="28">
         <v>73.12</v>
       </c>
-      <c r="J38" s="29">
+      <c r="J38" s="28">
         <v>74.97</v>
       </c>
-      <c r="K38" s="29">
+      <c r="K38" s="28">
         <v>65.290000000000006</v>
       </c>
-      <c r="L38" s="29">
+      <c r="L38" s="28">
         <v>69.040000000000006</v>
       </c>
-      <c r="M38" s="29">
+      <c r="M38" s="28">
         <v>44.17</v>
       </c>
-      <c r="N38" s="29">
+      <c r="N38" s="28">
         <v>3.81</v>
       </c>
-      <c r="O38" s="29">
+      <c r="O38" s="28">
         <v>3.44</v>
       </c>
-      <c r="P38" s="29">
+      <c r="P38" s="28">
         <v>5.38</v>
       </c>
-      <c r="Q38" s="29">
+      <c r="Q38" s="28">
         <v>5.41</v>
       </c>
-      <c r="R38" s="29">
+      <c r="R38" s="28">
         <v>5.09</v>
       </c>
-      <c r="S38" s="30"/>
-    </row>
-    <row r="39" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="28">
+      <c r="S38" s="29"/>
+    </row>
+    <row r="39" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="27">
         <v>2012</v>
       </c>
-      <c r="C39" s="28" t="s">
+      <c r="C39" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="29">
+      <c r="D39" s="28">
         <v>81.540000000000006</v>
       </c>
-      <c r="E39" s="29">
+      <c r="E39" s="28">
         <v>82.19</v>
       </c>
-      <c r="F39" s="29">
+      <c r="F39" s="28">
         <v>78.41</v>
       </c>
-      <c r="G39" s="29">
+      <c r="G39" s="28">
         <v>83.76</v>
       </c>
-      <c r="H39" s="29">
+      <c r="H39" s="28">
         <v>54.19</v>
       </c>
-      <c r="I39" s="29">
+      <c r="I39" s="28">
         <v>77.28</v>
       </c>
-      <c r="J39" s="29">
+      <c r="J39" s="28">
         <v>78.59</v>
       </c>
-      <c r="K39" s="29">
+      <c r="K39" s="28">
         <v>70.98</v>
       </c>
-      <c r="L39" s="29">
+      <c r="L39" s="28">
         <v>76.27</v>
       </c>
-      <c r="M39" s="29">
+      <c r="M39" s="28">
         <v>47.02</v>
       </c>
-      <c r="N39" s="29">
+      <c r="N39" s="28">
         <v>4.26</v>
       </c>
-      <c r="O39" s="29">
+      <c r="O39" s="28">
         <v>3.6</v>
       </c>
-      <c r="P39" s="29">
+      <c r="P39" s="28">
         <v>7.43</v>
       </c>
-      <c r="Q39" s="29">
+      <c r="Q39" s="28">
         <v>7.49</v>
       </c>
-      <c r="R39" s="29">
+      <c r="R39" s="28">
         <v>7.17</v>
       </c>
-      <c r="S39" s="30"/>
-    </row>
-    <row r="40" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="28">
+      <c r="S39" s="29"/>
+    </row>
+    <row r="40" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="27">
         <v>2012</v>
       </c>
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="29">
+      <c r="D40" s="28">
         <v>70.56</v>
       </c>
-      <c r="E40" s="29">
+      <c r="E40" s="28">
         <v>72.459999999999994</v>
       </c>
-      <c r="F40" s="29">
+      <c r="F40" s="28">
         <v>61.59</v>
       </c>
-      <c r="G40" s="29">
+      <c r="G40" s="28">
         <v>64.569999999999993</v>
       </c>
-      <c r="H40" s="29">
+      <c r="H40" s="28">
         <v>44.81</v>
       </c>
-      <c r="I40" s="29">
+      <c r="I40" s="28">
         <v>67.3</v>
       </c>
-      <c r="J40" s="29">
+      <c r="J40" s="28">
         <v>69.52</v>
       </c>
-      <c r="K40" s="29">
+      <c r="K40" s="28">
         <v>56.8</v>
       </c>
-      <c r="L40" s="29">
+      <c r="L40" s="28">
         <v>59.9</v>
       </c>
-      <c r="M40" s="29">
+      <c r="M40" s="28">
         <v>39.369999999999997</v>
       </c>
-      <c r="N40" s="29">
+      <c r="N40" s="28">
         <v>3.26</v>
       </c>
-      <c r="O40" s="29">
+      <c r="O40" s="28">
         <v>2.94</v>
       </c>
-      <c r="P40" s="29">
+      <c r="P40" s="28">
         <v>4.79</v>
       </c>
-      <c r="Q40" s="29">
+      <c r="Q40" s="28">
         <v>4.67</v>
       </c>
-      <c r="R40" s="29">
+      <c r="R40" s="28">
         <v>5.44</v>
       </c>
-      <c r="S40" s="30"/>
-    </row>
-    <row r="41" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="28">
+      <c r="S40" s="29"/>
+    </row>
+    <row r="41" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="27">
         <v>2012</v>
       </c>
-      <c r="C41" s="28" t="s">
+      <c r="C41" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="29">
+      <c r="D41" s="28">
         <v>76.09</v>
       </c>
-      <c r="E41" s="29">
+      <c r="E41" s="28">
         <v>77.37</v>
       </c>
-      <c r="F41" s="29">
+      <c r="F41" s="28">
         <v>70</v>
       </c>
-      <c r="G41" s="29">
+      <c r="G41" s="28">
         <v>73.989999999999995</v>
       </c>
-      <c r="H41" s="29">
+      <c r="H41" s="28">
         <v>49.93</v>
       </c>
-      <c r="I41" s="29">
+      <c r="I41" s="28">
         <v>72.319999999999993</v>
       </c>
-      <c r="J41" s="29">
+      <c r="J41" s="28">
         <v>74.099999999999994</v>
       </c>
-      <c r="K41" s="29">
+      <c r="K41" s="28">
         <v>63.89</v>
       </c>
-      <c r="L41" s="29">
+      <c r="L41" s="28">
         <v>67.94</v>
       </c>
-      <c r="M41" s="29">
+      <c r="M41" s="28">
         <v>43.54</v>
       </c>
-      <c r="N41" s="29">
+      <c r="N41" s="28">
         <v>3.76</v>
       </c>
-      <c r="O41" s="29">
+      <c r="O41" s="28">
         <v>3.27</v>
       </c>
-      <c r="P41" s="29">
+      <c r="P41" s="28">
         <v>6.11</v>
       </c>
-      <c r="Q41" s="29">
+      <c r="Q41" s="28">
         <v>6.06</v>
       </c>
-      <c r="R41" s="29">
+      <c r="R41" s="28">
         <v>6.38</v>
       </c>
-      <c r="S41" s="30"/>
-    </row>
-    <row r="42" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="28">
+      <c r="S41" s="29"/>
+    </row>
+    <row r="42" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="27">
         <v>2011</v>
       </c>
-      <c r="C42" s="28" t="s">
+      <c r="C42" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="29">
+      <c r="D42" s="28">
         <v>81.680000000000007</v>
       </c>
-      <c r="E42" s="29">
+      <c r="E42" s="28">
         <v>82.3</v>
       </c>
-      <c r="F42" s="29">
+      <c r="F42" s="28">
         <v>78.599999999999994</v>
       </c>
-      <c r="G42" s="29">
+      <c r="G42" s="28">
         <v>84.19</v>
       </c>
-      <c r="H42" s="29">
+      <c r="H42" s="28">
         <v>54.02</v>
       </c>
-      <c r="I42" s="29">
+      <c r="I42" s="28">
         <v>77.150000000000006</v>
       </c>
-      <c r="J42" s="29">
+      <c r="J42" s="28">
         <v>78.44</v>
       </c>
-      <c r="K42" s="29">
+      <c r="K42" s="28">
         <v>70.8</v>
       </c>
-      <c r="L42" s="29">
+      <c r="L42" s="28">
         <v>75.84</v>
       </c>
-      <c r="M42" s="29">
+      <c r="M42" s="28">
         <v>48.64</v>
       </c>
-      <c r="N42" s="29">
+      <c r="N42" s="28">
         <v>4.53</v>
       </c>
-      <c r="O42" s="29">
+      <c r="O42" s="28">
         <v>3.87</v>
       </c>
-      <c r="P42" s="29">
+      <c r="P42" s="28">
         <v>7.8</v>
       </c>
-      <c r="Q42" s="29">
+      <c r="Q42" s="28">
         <v>8.35</v>
       </c>
-      <c r="R42" s="29">
+      <c r="R42" s="28">
         <v>5.38</v>
       </c>
-      <c r="S42" s="30"/>
-    </row>
-    <row r="43" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="28">
+      <c r="S42" s="29"/>
+    </row>
+    <row r="43" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="27">
         <v>2011</v>
       </c>
-      <c r="C43" s="28" t="s">
+      <c r="C43" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D43" s="29">
+      <c r="D43" s="28">
         <v>70.569999999999993</v>
       </c>
-      <c r="E43" s="29">
+      <c r="E43" s="28">
         <v>72.459999999999994</v>
       </c>
-      <c r="F43" s="29">
+      <c r="F43" s="28">
         <v>61.52</v>
       </c>
-      <c r="G43" s="29">
+      <c r="G43" s="28">
         <v>64</v>
       </c>
-      <c r="H43" s="29">
+      <c r="H43" s="28">
         <v>47.35</v>
       </c>
-      <c r="I43" s="29">
+      <c r="I43" s="28">
         <v>66.63</v>
       </c>
-      <c r="J43" s="29">
+      <c r="J43" s="28">
         <v>68.819999999999993</v>
       </c>
-      <c r="K43" s="29">
+      <c r="K43" s="28">
         <v>56.2</v>
       </c>
-      <c r="L43" s="29">
+      <c r="L43" s="28">
         <v>58.27</v>
       </c>
-      <c r="M43" s="29">
+      <c r="M43" s="28">
         <v>44.41</v>
       </c>
-      <c r="N43" s="29">
+      <c r="N43" s="28">
         <v>3.93</v>
       </c>
-      <c r="O43" s="29">
+      <c r="O43" s="28">
         <v>3.65</v>
       </c>
-      <c r="P43" s="29">
+      <c r="P43" s="28">
         <v>5.32</v>
       </c>
-      <c r="Q43" s="29">
+      <c r="Q43" s="28">
         <v>5.73</v>
       </c>
-      <c r="R43" s="29">
+      <c r="R43" s="28">
         <v>2.94</v>
       </c>
-      <c r="S43" s="30"/>
-    </row>
-    <row r="44" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="28">
+      <c r="S43" s="29"/>
+    </row>
+    <row r="44" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="27">
         <v>2011</v>
       </c>
-      <c r="C44" s="28" t="s">
+      <c r="C44" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D44" s="29">
+      <c r="D44" s="28">
         <v>76.150000000000006</v>
       </c>
-      <c r="E44" s="29">
+      <c r="E44" s="28">
         <v>77.42</v>
       </c>
-      <c r="F44" s="29">
+      <c r="F44" s="28">
         <v>69.98</v>
       </c>
-      <c r="G44" s="29">
+      <c r="G44" s="28">
         <v>73.77</v>
       </c>
-      <c r="H44" s="29">
+      <c r="H44" s="28">
         <v>51.02</v>
       </c>
-      <c r="I44" s="29">
+      <c r="I44" s="28">
         <v>71.92</v>
       </c>
-      <c r="J44" s="29">
+      <c r="J44" s="28">
         <v>73.66</v>
       </c>
-      <c r="K44" s="29">
+      <c r="K44" s="28">
         <v>63.43</v>
       </c>
-      <c r="L44" s="29">
+      <c r="L44" s="28">
         <v>66.77</v>
       </c>
-      <c r="M44" s="29">
+      <c r="M44" s="28">
         <v>46.74</v>
       </c>
-      <c r="N44" s="29">
+      <c r="N44" s="28">
         <v>4.2300000000000004</v>
       </c>
-      <c r="O44" s="29">
+      <c r="O44" s="28">
         <v>3.76</v>
       </c>
-      <c r="P44" s="29">
+      <c r="P44" s="28">
         <v>6.55</v>
       </c>
-      <c r="Q44" s="29">
+      <c r="Q44" s="28">
         <v>7</v>
       </c>
-      <c r="R44" s="29">
+      <c r="R44" s="28">
         <v>4.28</v>
       </c>
-      <c r="S44" s="30"/>
-    </row>
-    <row r="45" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="28">
+      <c r="S44" s="29"/>
+    </row>
+    <row r="45" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="27">
         <v>2005</v>
       </c>
-      <c r="C45" s="28" t="s">
+      <c r="C45" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D45" s="29">
+      <c r="D45" s="28">
         <v>79.62</v>
       </c>
-      <c r="E45" s="29">
+      <c r="E45" s="28">
         <v>80.349999999999994</v>
       </c>
-      <c r="F45" s="29">
+      <c r="F45" s="28">
         <v>75.94</v>
       </c>
-      <c r="G45" s="29">
+      <c r="G45" s="28">
         <v>78.64</v>
       </c>
-      <c r="H45" s="29">
+      <c r="H45" s="28">
         <v>60.46</v>
       </c>
-      <c r="I45" s="29">
+      <c r="I45" s="28">
         <v>70.92</v>
       </c>
-      <c r="J45" s="29">
+      <c r="J45" s="28">
         <v>72.95</v>
       </c>
-      <c r="K45" s="29">
+      <c r="K45" s="28">
         <v>60.69</v>
       </c>
-      <c r="L45" s="29">
+      <c r="L45" s="28">
         <v>63.07</v>
       </c>
-      <c r="M45" s="29">
+      <c r="M45" s="28">
         <v>47.04</v>
       </c>
-      <c r="N45" s="29">
+      <c r="N45" s="28">
         <v>8.69</v>
       </c>
-      <c r="O45" s="29">
+      <c r="O45" s="28">
         <v>7.39</v>
       </c>
-      <c r="P45" s="29">
+      <c r="P45" s="28">
         <v>15.25</v>
       </c>
-      <c r="Q45" s="29">
+      <c r="Q45" s="28">
         <v>15.57</v>
       </c>
-      <c r="R45" s="29">
+      <c r="R45" s="28">
         <v>13.42</v>
       </c>
-      <c r="S45" s="30"/>
-    </row>
-    <row r="46" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="28">
+      <c r="S45" s="29"/>
+    </row>
+    <row r="46" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="27">
         <v>2005</v>
       </c>
-      <c r="C46" s="28" t="s">
+      <c r="C46" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D46" s="29">
+      <c r="D46" s="28">
         <v>64.12</v>
       </c>
-      <c r="E46" s="29">
+      <c r="E46" s="28">
         <v>65.97</v>
       </c>
-      <c r="F46" s="29">
+      <c r="F46" s="28">
         <v>54.55</v>
       </c>
-      <c r="G46" s="29">
+      <c r="G46" s="28">
         <v>55.86</v>
       </c>
-      <c r="H46" s="29">
+      <c r="H46" s="28">
         <v>44.98</v>
       </c>
-      <c r="I46" s="29">
+      <c r="I46" s="28">
         <v>57.68</v>
       </c>
-      <c r="J46" s="29">
+      <c r="J46" s="28">
         <v>60.09</v>
       </c>
-      <c r="K46" s="29">
+      <c r="K46" s="28">
         <v>45.23</v>
       </c>
-      <c r="L46" s="29">
+      <c r="L46" s="28">
         <v>46.05</v>
       </c>
-      <c r="M46" s="29">
+      <c r="M46" s="28">
         <v>39.26</v>
       </c>
-      <c r="N46" s="29">
+      <c r="N46" s="28">
         <v>6.44</v>
       </c>
-      <c r="O46" s="29">
+      <c r="O46" s="28">
         <v>5.89</v>
       </c>
-      <c r="P46" s="29">
+      <c r="P46" s="28">
         <v>9.32</v>
       </c>
-      <c r="Q46" s="29">
+      <c r="Q46" s="28">
         <v>9.81</v>
       </c>
-      <c r="R46" s="29">
+      <c r="R46" s="28">
         <v>5.71</v>
       </c>
-      <c r="S46" s="30"/>
-    </row>
-    <row r="47" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="28">
+      <c r="S46" s="29"/>
+    </row>
+    <row r="47" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="27">
         <v>2005</v>
       </c>
-      <c r="C47" s="28" t="s">
+      <c r="C47" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="29">
+      <c r="D47" s="28">
         <v>71.94</v>
       </c>
-      <c r="E47" s="29">
+      <c r="E47" s="28">
         <v>73.209999999999994</v>
       </c>
-      <c r="F47" s="29">
+      <c r="F47" s="28">
         <v>65.45</v>
       </c>
-      <c r="G47" s="29">
+      <c r="G47" s="28">
         <v>67.290000000000006</v>
       </c>
-      <c r="H47" s="29">
+      <c r="H47" s="28">
         <v>53.67</v>
       </c>
-      <c r="I47" s="29">
+      <c r="I47" s="28">
         <v>64.36</v>
       </c>
-      <c r="J47" s="29">
+      <c r="J47" s="28">
         <v>66.56</v>
       </c>
-      <c r="K47" s="29">
+      <c r="K47" s="28">
         <v>53.11</v>
       </c>
-      <c r="L47" s="29">
+      <c r="L47" s="28">
         <v>54.59</v>
       </c>
-      <c r="M47" s="29">
+      <c r="M47" s="28">
         <v>43.63</v>
       </c>
-      <c r="N47" s="29">
+      <c r="N47" s="28">
         <v>7.58</v>
       </c>
-      <c r="O47" s="29">
+      <c r="O47" s="28">
         <v>6.65</v>
       </c>
-      <c r="P47" s="29">
+      <c r="P47" s="28">
         <v>12.34</v>
       </c>
-      <c r="Q47" s="29">
+      <c r="Q47" s="28">
         <v>12.7</v>
       </c>
-      <c r="R47" s="29">
+      <c r="R47" s="28">
         <v>10.039999999999999</v>
       </c>
-      <c r="S47" s="30"/>
+      <c r="S47" s="29"/>
     </row>
     <row r="48" spans="2:19" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B48" s="28"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-      <c r="H48" s="31"/>
-      <c r="I48" s="31"/>
-      <c r="J48" s="31"/>
-      <c r="K48" s="31"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="30"/>
+      <c r="K48" s="30"/>
       <c r="N48" s="7"/>
     </row>
     <row r="49" spans="2:14" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B49" s="32"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="33"/>
-      <c r="E49" s="33"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="33"/>
-      <c r="H49" s="33"/>
-      <c r="I49" s="33"/>
-      <c r="J49" s="33"/>
-      <c r="K49" s="33"/>
-      <c r="N49" s="34"/>
-    </row>
-    <row r="50" spans="2:14" s="36" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="35" t="s">
+      <c r="B49" s="31"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="32"/>
+      <c r="J49" s="32"/>
+      <c r="K49" s="32"/>
+      <c r="N49" s="33"/>
+    </row>
+    <row r="50" spans="2:14" s="35" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C50" s="35"/>
-      <c r="D50" s="35"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="35"/>
-      <c r="H50" s="35"/>
-      <c r="I50" s="35"/>
-      <c r="J50" s="35"/>
-      <c r="K50" s="35"/>
-      <c r="N50" s="37"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="34"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="34"/>
+      <c r="G50" s="34"/>
+      <c r="H50" s="34"/>
+      <c r="I50" s="34"/>
+      <c r="J50" s="34"/>
+      <c r="K50" s="34"/>
+      <c r="N50" s="36"/>
     </row>
     <row r="51" spans="2:14" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B51" s="33" t="s">
+      <c r="B51" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="33"/>
-      <c r="D51" s="33"/>
-      <c r="E51" s="33"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="33"/>
-      <c r="H51" s="33"/>
-      <c r="I51" s="33"/>
-      <c r="J51" s="33"/>
-      <c r="K51" s="33"/>
-      <c r="N51" s="34"/>
-    </row>
-    <row r="52" spans="2:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="38" t="s">
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="32"/>
+      <c r="J51" s="32"/>
+      <c r="K51" s="32"/>
+      <c r="N51" s="33"/>
+    </row>
+    <row r="52" spans="2:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="38"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="38"/>
-      <c r="F52" s="38"/>
-      <c r="G52" s="38"/>
-      <c r="H52" s="38"/>
-      <c r="I52" s="38"/>
-      <c r="J52" s="38"/>
-      <c r="K52" s="38"/>
-    </row>
-    <row r="53" spans="2:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="38" t="s">
+      <c r="C52" s="37"/>
+      <c r="D52" s="37"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="37"/>
+      <c r="J52" s="37"/>
+      <c r="K52" s="37"/>
+    </row>
+    <row r="53" spans="2:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C53" s="38"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="38"/>
-      <c r="J53" s="38"/>
-      <c r="K53" s="38"/>
-    </row>
-    <row r="54" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="39" t="s">
+      <c r="C53" s="37"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="37"/>
+      <c r="J53" s="37"/>
+      <c r="K53" s="37"/>
+    </row>
+    <row r="54" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C54" s="40"/>
-      <c r="D54" s="40"/>
-      <c r="E54" s="40"/>
-      <c r="F54" s="40"/>
-      <c r="G54" s="40"/>
-      <c r="H54" s="40"/>
-      <c r="I54" s="40"/>
-      <c r="J54" s="40"/>
-      <c r="K54" s="40"/>
-    </row>
-    <row r="55" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="40"/>
-      <c r="C55" s="40"/>
-      <c r="D55" s="40"/>
-      <c r="E55" s="40"/>
-      <c r="F55" s="40"/>
-      <c r="G55" s="40"/>
-      <c r="H55" s="40"/>
-      <c r="I55" s="40"/>
-      <c r="J55" s="40"/>
-      <c r="K55" s="40"/>
-    </row>
-    <row r="56" spans="2:14" s="36" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="41" t="s">
+      <c r="C54" s="39"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="39"/>
+      <c r="I54" s="39"/>
+      <c r="J54" s="39"/>
+      <c r="K54" s="39"/>
+    </row>
+    <row r="55" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="39"/>
+      <c r="C55" s="39"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="39"/>
+      <c r="H55" s="39"/>
+      <c r="I55" s="39"/>
+      <c r="J55" s="39"/>
+      <c r="K55" s="39"/>
+    </row>
+    <row r="56" spans="2:14" s="35" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="42"/>
-      <c r="D56" s="42"/>
-      <c r="E56" s="42"/>
-      <c r="F56" s="42"/>
-      <c r="G56" s="42"/>
-      <c r="H56" s="42"/>
-      <c r="I56" s="42"/>
-      <c r="J56" s="42"/>
-      <c r="K56" s="42"/>
-    </row>
-    <row r="57" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="2:14" s="36" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="41" t="s">
+      <c r="C56" s="41"/>
+      <c r="D56" s="41"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="41"/>
+      <c r="H56" s="41"/>
+      <c r="I56" s="41"/>
+      <c r="J56" s="41"/>
+      <c r="K56" s="41"/>
+    </row>
+    <row r="57" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="2:14" s="35" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C58" s="42"/>
-      <c r="D58" s="42"/>
-      <c r="E58" s="42"/>
-      <c r="F58" s="42"/>
-      <c r="G58" s="42"/>
-      <c r="H58" s="42"/>
-      <c r="I58" s="42"/>
-      <c r="J58" s="42"/>
-      <c r="K58" s="42"/>
-    </row>
-    <row r="59" spans="2:14" s="36" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="41" t="s">
+      <c r="C58" s="41"/>
+      <c r="D58" s="41"/>
+      <c r="E58" s="41"/>
+      <c r="F58" s="41"/>
+      <c r="G58" s="41"/>
+      <c r="H58" s="41"/>
+      <c r="I58" s="41"/>
+      <c r="J58" s="41"/>
+      <c r="K58" s="41"/>
+    </row>
+    <row r="59" spans="2:14" s="35" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C59" s="42"/>
-      <c r="D59" s="42"/>
-      <c r="E59" s="42"/>
-      <c r="F59" s="42"/>
-      <c r="G59" s="42"/>
-      <c r="H59" s="42"/>
-      <c r="I59" s="42"/>
-      <c r="J59" s="42"/>
-      <c r="K59" s="42"/>
-    </row>
-    <row r="60" spans="2:14" s="36" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="41" t="s">
+      <c r="C59" s="41"/>
+      <c r="D59" s="41"/>
+      <c r="E59" s="41"/>
+      <c r="F59" s="41"/>
+      <c r="G59" s="41"/>
+      <c r="H59" s="41"/>
+      <c r="I59" s="41"/>
+      <c r="J59" s="41"/>
+      <c r="K59" s="41"/>
+    </row>
+    <row r="60" spans="2:14" s="35" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C60" s="42"/>
-      <c r="D60" s="42"/>
-      <c r="E60" s="42"/>
-      <c r="F60" s="42"/>
-      <c r="G60" s="42"/>
-      <c r="H60" s="42"/>
-      <c r="I60" s="42"/>
-      <c r="J60" s="42"/>
-      <c r="K60" s="42"/>
-    </row>
-    <row r="61" spans="2:14" s="36" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="43" t="s">
+      <c r="C60" s="41"/>
+      <c r="D60" s="41"/>
+      <c r="E60" s="41"/>
+      <c r="F60" s="41"/>
+      <c r="G60" s="41"/>
+      <c r="H60" s="41"/>
+      <c r="I60" s="41"/>
+      <c r="J60" s="41"/>
+      <c r="K60" s="41"/>
+    </row>
+    <row r="61" spans="2:14" s="35" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C61" s="42"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="42"/>
-      <c r="F61" s="42"/>
-      <c r="G61" s="42"/>
-      <c r="H61" s="42"/>
-      <c r="I61" s="42"/>
-      <c r="J61" s="42"/>
-      <c r="K61" s="42"/>
+      <c r="C61" s="41"/>
+      <c r="D61" s="41"/>
+      <c r="E61" s="41"/>
+      <c r="F61" s="41"/>
+      <c r="G61" s="41"/>
+      <c r="H61" s="41"/>
+      <c r="I61" s="41"/>
+      <c r="J61" s="41"/>
+      <c r="K61" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -3220,8 +3220,8 @@
     <mergeCell ref="J7:M7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B61" r:id="rId1" xr:uid="{E22D39AF-A5C8-4285-A905-B0EBF2430775}"/>
-    <hyperlink ref="B54" r:id="rId2" xr:uid="{A5AA1DEC-E7D5-434E-94FB-44AEB5058569}"/>
+    <hyperlink ref="B61" r:id="rId1" xr:uid="{2945A0A5-357C-4E33-B482-746C187FF698}"/>
+    <hyperlink ref="B54" r:id="rId2" xr:uid="{34971897-4F58-4475-B080-42E31F9728AF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>